<commit_message>
Manta Time/Space Match Attempt
</commit_message>
<xml_diff>
--- a/Accuracy Comparison.xlsx
+++ b/Accuracy Comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Google Drive/Georgia Tech Notes/Capstone/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE2A8F0C-D490-654A-918D-EE93118C5FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFECA4F-60ED-9D46-9763-81222DDDB5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="37400" windowHeight="21100" xr2:uid="{8A8B95BA-E442-C945-92A2-F70F81568E72}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="32560" windowHeight="20500" xr2:uid="{8A8B95BA-E442-C945-92A2-F70F81568E72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1173,16 +1173,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1510,7 +1510,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>